<commit_message>
updated foreign keys for all the tables
</commit_message>
<xml_diff>
--- a/public/files/Employee_Data.xlsx
+++ b/public/files/Employee_Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\groemp\public\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp_docs\htdocs\groemp\public\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{44D466B6-551D-4BEE-94BF-ADDBA944DCC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F9FB91-8587-4BF9-A769-5C5B8B790758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F78553D5-1CAD-42B2-AFF4-4AB8819A8D2C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>pan_number</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>benefit_amount</t>
+  </si>
+  <si>
+    <t>employee_id</t>
   </si>
 </sst>
 </file>
@@ -406,34 +409,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E73063-846E-4BBF-AF89-1A12345910E0}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>